<commit_message>
TA can read TagsConfig
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/TAOrderExample.xlsx
+++ b/AD-EYE/TA/Configurations/TAOrderExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39330AE-341F-4571-86F4-4AD7A3530BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A23BDA-352B-48F5-8B7D-0072C25D23E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12396" yWindow="2376" windowWidth="14724" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8250" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAOrderExample" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>FolderExpName</t>
   </si>
@@ -52,16 +52,16 @@
     <t>SimulinkConfigExample.xlsx</t>
   </si>
   <si>
-    <t>SimulinkConfigTemplate.xlsx</t>
-  </si>
-  <si>
     <t>TagsConfig</t>
   </si>
   <si>
     <t>SHHConfig</t>
   </si>
   <si>
-    <t>ssh</t>
+    <t>Configurations/SSHConfig.csv</t>
+  </si>
+  <si>
+    <t>fog=true/fog_visible=85</t>
   </si>
 </sst>
 </file>
@@ -902,83 +902,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.453125" customWidth="1"/>
+    <col min="2" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature to read TagsConfig is more robust
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/TAOrderExample.xlsx
+++ b/AD-EYE/TA/Configurations/TAOrderExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A23BDA-352B-48F5-8B7D-0072C25D23E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC94A95-885F-40F5-A848-00247F479838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="8250" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>FolderExpName</t>
   </si>
@@ -902,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,47 +915,62 @@
     <col min="3" max="3" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -963,11 +978,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the matlab srcipt which handle the database connection
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/TAOrderExample.xlsx
+++ b/AD-EYE/TA/Configurations/TAOrderExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC94A95-885F-40F5-A848-00247F479838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2659C7D7-99E9-4E08-9428-965770E827A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8250" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="11040" windowWidth="28800" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAOrderExample" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>FolderExpName</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Configurations/SSHConfig.csv</t>
-  </si>
-  <si>
-    <t>fog=true/fog_visible=85</t>
   </si>
 </sst>
 </file>
@@ -904,14 +901,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="30.6328125" customWidth="1"/>
+    <col min="2" max="2" width="52.6328125" customWidth="1"/>
     <col min="3" max="3" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -974,9 +971,6 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">

</xml_diff>

<commit_message>
Renamed Base_Map to Base_World in TAOrder files
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/TAOrderExample.xlsx
+++ b/AD-EYE/TA/Configurations/TAOrderExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2659C7D7-99E9-4E08-9428-965770E827A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49233537-FCD7-4FC8-A199-6134FD0A81EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11040" windowWidth="28800" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6372" yWindow="3600" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TAOrderExample" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>FolderExpName</t>
   </si>
   <si>
-    <t>W01_Base_Map/Simulation</t>
-  </si>
-  <si>
     <t>PrescanExpName</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>Configurations/SSHConfig.csv</t>
+  </si>
+  <si>
+    <t>W01_Base_World/Simulation</t>
   </si>
 </sst>
 </file>
@@ -902,85 +902,85 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.453125" customWidth="1"/>
-    <col min="2" max="2" width="52.6328125" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>